<commit_message>
Adding PIB feature generation algorithm
</commit_message>
<xml_diff>
--- a/evaluation/train_test_data.xlsx
+++ b/evaluation/train_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameenislam/Documents/MSc_Project/code.nosync/chbmit-seizure-prediction/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BB4A35-7BB6-D749-9BDA-567101AFA3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9276D732-4365-6C49-B9AA-5182769EEB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37340" yWindow="5060" windowWidth="28040" windowHeight="17440" xr2:uid="{0C40A520-936C-D94E-A26D-68C33228D3D9}"/>
   </bookViews>
@@ -610,9 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0D9E85-EE3C-CA4A-A123-B4CA2E9C6277}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Extending chb06 interictal test set
</commit_message>
<xml_diff>
--- a/evaluation/train_test_data.xlsx
+++ b/evaluation/train_test_data.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameenislam/Documents/MSc_Project/code.nosync/chbmit-seizure-prediction/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9276D732-4365-6C49-B9AA-5182769EEB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBDC063-0289-D34D-A48E-24A502BF452E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37340" yWindow="5060" windowWidth="28040" windowHeight="17440" xr2:uid="{0C40A520-936C-D94E-A26D-68C33228D3D9}"/>
+    <workbookView xWindow="540" yWindow="500" windowWidth="21920" windowHeight="19920" xr2:uid="{0C40A520-936C-D94E-A26D-68C33228D3D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$51</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="77">
   <si>
     <t>Case</t>
   </si>
@@ -224,6 +227,48 @@
   </si>
   <si>
     <t>chb06_08.edf</t>
+  </si>
+  <si>
+    <t>chb01_09.edf</t>
+  </si>
+  <si>
+    <t>chb01_10.edf</t>
+  </si>
+  <si>
+    <t>chb01_11.edf</t>
+  </si>
+  <si>
+    <t>chb01_12.edf</t>
+  </si>
+  <si>
+    <t>chb01_13.edf</t>
+  </si>
+  <si>
+    <t>chb01_14.edf</t>
+  </si>
+  <si>
+    <t>chb01_17.edf</t>
+  </si>
+  <si>
+    <t>chb01_19.edf</t>
+  </si>
+  <si>
+    <t>chb01_20.edf</t>
+  </si>
+  <si>
+    <t>chb06_12.edf</t>
+  </si>
+  <si>
+    <t>chb06_14.edf</t>
+  </si>
+  <si>
+    <t>chb06_15.edf</t>
+  </si>
+  <si>
+    <t>chb06_16.edf</t>
+  </si>
+  <si>
+    <t>chb06_17.edf</t>
   </si>
 </sst>
 </file>
@@ -608,9 +653,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0D9E85-EE3C-CA4A-A123-B4CA2E9C6277}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1232,13 +1279,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
         <v>30</v>
@@ -1255,13 +1302,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
         <v>30</v>
@@ -1278,13 +1325,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1301,10 +1348,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
@@ -1324,10 +1371,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -1347,10 +1394,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
@@ -1370,13 +1417,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
         <v>30</v>
@@ -1393,13 +1440,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
         <v>30</v>
@@ -1416,13 +1463,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
         <v>30</v>
@@ -1439,13 +1486,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
         <v>30</v>
@@ -1462,13 +1509,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
         <v>30</v>
@@ -1485,24 +1532,348 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f>900*2</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <f>900*2</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B46" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C37" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
         <v>900</v>
       </c>
     </row>

</xml_diff>